<commit_message>
Add achievements, Discord reports, and per-attack avg stars
</commit_message>
<xml_diff>
--- a/clash_wars.xlsx
+++ b/clash_wars.xlsx
@@ -707,7 +707,7 @@
         <v>2</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -791,7 +791,7 @@
         <v>2</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
@@ -875,7 +875,7 @@
         <v>2</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -1001,7 +1001,7 @@
         <v>2</v>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27">
@@ -1043,7 +1043,7 @@
         <v>2</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29">
@@ -1085,7 +1085,7 @@
         <v>2</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
@@ -1148,7 +1148,7 @@
         <v>2</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
@@ -1211,7 +1211,7 @@
         <v>2</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
@@ -4773,7 +4773,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5436,13 +5436,13 @@
         <v>21</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
@@ -5451,7 +5451,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -5486,22 +5486,22 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Anon</t>
+          <t>Downsy m8</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>#2VRP9CJY</t>
+          <t>#PYR0JQC</t>
         </is>
       </c>
       <c r="H11" t="n">
         <v>18</v>
       </c>
       <c r="I11" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="J11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" t="n">
         <v>3</v>
@@ -5566,7 +5566,7 @@
         <v>12</v>
       </c>
       <c r="J12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K12" t="n">
         <v>3</v>
@@ -5616,37 +5616,37 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>«#PATRICK#»</t>
+          <t>Anon</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>#8R8R0GL9</t>
+          <t>#2VRP9CJY</t>
         </is>
       </c>
       <c r="H13" t="n">
         <v>18</v>
       </c>
       <c r="I13" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
@@ -5681,37 +5681,37 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Frodo</t>
+          <t>«#PATRICK#»</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>#282Q98Y9J</t>
+          <t>#8R8R0GL9</t>
         </is>
       </c>
       <c r="H14" t="n">
         <v>18</v>
       </c>
       <c r="I14" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="J14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
@@ -5761,7 +5761,7 @@
         <v>17</v>
       </c>
       <c r="J15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K15" t="n">
         <v>3</v>
@@ -5811,37 +5811,37 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>stars2</t>
+          <t>Frodo</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>#YJC80V2QC</t>
+          <t>#282Q98Y9J</t>
         </is>
       </c>
       <c r="H16" t="n">
+        <v>18</v>
+      </c>
+      <c r="I16" t="n">
         <v>17</v>
       </c>
-      <c r="I16" t="n">
-        <v>29</v>
-      </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -5876,28 +5876,28 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Innersinn</t>
+          <t>stars2</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>#9UUG9GPC</t>
+          <t>#YJC80V2QC</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I17" t="n">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="M17" t="inlineStr">
         <is>
@@ -5906,7 +5906,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -5941,32 +5941,32 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>platypus</t>
+          <t>stars2</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>#VQUQ8992</t>
+          <t>#YJC80V2QC</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I18" t="n">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="J18" t="n">
+        <v>2</v>
+      </c>
+      <c r="K18" t="n">
         <v>1</v>
       </c>
-      <c r="K18" t="n">
-        <v>3</v>
-      </c>
       <c r="L18" t="n">
-        <v>100</v>
+        <v>23</v>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
@@ -6006,32 +6006,32 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>BlueberyPancake</t>
+          <t>Innersinn</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>#G2PQRR0QV</t>
+          <t>#9UUG9GPC</t>
         </is>
       </c>
       <c r="H19" t="n">
         <v>18</v>
       </c>
       <c r="I19" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J19" t="n">
         <v>1</v>
       </c>
       <c r="K19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L19" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
@@ -6071,32 +6071,32 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>BlueberyPancake</t>
+          <t>Innersinn</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>#G2PQRR0QV</t>
+          <t>#9UUG9GPC</t>
         </is>
       </c>
       <c r="H20" t="n">
         <v>18</v>
       </c>
       <c r="I20" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J20" t="n">
         <v>2</v>
       </c>
       <c r="K20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L20" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
@@ -6136,37 +6136,37 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Z E T S U SKY⚡</t>
+          <t>platypus</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>#2LVYUPJ9Q</t>
+          <t>#VQUQ8992</t>
         </is>
       </c>
       <c r="H21" t="n">
         <v>18</v>
       </c>
       <c r="I21" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L21" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
@@ -6201,19 +6201,19 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>100% dado</t>
+          <t>BlueberyPancake</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>#8G89CPJVU</t>
+          <t>#G2PQRR0QV</t>
         </is>
       </c>
       <c r="H22" t="n">
         <v>18</v>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J22" t="n">
         <v>1</v>
@@ -6266,32 +6266,32 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>100% dado</t>
+          <t>BlueberyPancake</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>#8G89CPJVU</t>
+          <t>#G2PQRR0QV</t>
         </is>
       </c>
       <c r="H23" t="n">
         <v>18</v>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J23" t="n">
         <v>2</v>
       </c>
       <c r="K23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L23" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
@@ -6331,19 +6331,19 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>savage slayer</t>
+          <t>Z E T S U SKY⚡</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>#YGY8R0YV8</t>
+          <t>#2LVYUPJ9Q</t>
         </is>
       </c>
       <c r="H24" t="n">
         <v>18</v>
       </c>
       <c r="I24" t="n">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="J24" t="n">
         <v>0</v>
@@ -6396,37 +6396,37 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>abhi</t>
+          <t>100% dado</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>#P8Y9JR8CP</t>
+          <t>#8G89CPJVU</t>
         </is>
       </c>
       <c r="H25" t="n">
         <v>18</v>
       </c>
       <c r="I25" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="J25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L25" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
@@ -6461,37 +6461,37 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Krunal</t>
+          <t>100% dado</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>#8VC29JPJP</t>
+          <t>#8G89CPJVU</t>
         </is>
       </c>
       <c r="H26" t="n">
         <v>18</v>
       </c>
       <c r="I26" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="J26" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K26" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L26" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
@@ -6526,37 +6526,37 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>GhosTAngeL</t>
+          <t>savage slayer</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>#YQ8V829CQ</t>
+          <t>#YGY8R0YV8</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I27" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="J27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L27" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
@@ -6591,28 +6591,28 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>TN • Raiden</t>
+          <t>savage slayer</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>#GV90C0LU</t>
+          <t>#YGY8R0YV8</t>
         </is>
       </c>
       <c r="H28" t="n">
         <v>18</v>
       </c>
       <c r="I28" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="J28" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K28" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L28" t="n">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="M28" t="inlineStr">
         <is>
@@ -6621,7 +6621,7 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
@@ -6656,28 +6656,28 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Mr Owl</t>
+          <t>abhi</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>#LQ8CU8GPU</t>
+          <t>#P8Y9JR8CP</t>
         </is>
       </c>
       <c r="H29" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I29" t="n">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L29" t="n">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="M29" t="inlineStr">
         <is>
@@ -6686,7 +6686,7 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
@@ -6721,22 +6721,22 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>100% Amos</t>
+          <t>abhi</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>#LYGLRCQCR</t>
+          <t>#P8Y9JR8CP</t>
         </is>
       </c>
       <c r="H30" t="n">
         <v>18</v>
       </c>
       <c r="I30" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K30" t="n">
         <v>3</v>
@@ -6786,28 +6786,28 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>100% Amos</t>
+          <t>Krunal</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>#LYGLRCQCR</t>
+          <t>#8VC29JPJP</t>
         </is>
       </c>
       <c r="H31" t="n">
         <v>18</v>
       </c>
       <c r="I31" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="J31" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L31" t="n">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="M31" t="inlineStr">
         <is>
@@ -6816,7 +6816,7 @@
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
@@ -6851,19 +6851,19 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>LittleSinn</t>
+          <t>GhosTAngeL</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>#YGV99UU</t>
+          <t>#YQ8V829CQ</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I32" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J32" t="n">
         <v>0</v>
@@ -6916,19 +6916,19 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>100% Titan</t>
+          <t>TN • Raiden</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>#YJVLJG8U</t>
+          <t>#GV90C0LU</t>
         </is>
       </c>
       <c r="H33" t="n">
         <v>18</v>
       </c>
       <c r="I33" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J33" t="n">
         <v>1</v>
@@ -6981,19 +6981,19 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>100% Titan</t>
+          <t>TN • Raiden</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>#YJVLJG8U</t>
+          <t>#GV90C0LU</t>
         </is>
       </c>
       <c r="H34" t="n">
         <v>18</v>
       </c>
       <c r="I34" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J34" t="n">
         <v>2</v>
@@ -7046,28 +7046,28 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>acowboy7</t>
+          <t>Mr Owl</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>#9L0C0C82</t>
+          <t>#LQ8CU8GPU</t>
         </is>
       </c>
       <c r="H35" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I35" t="n">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="J35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L35" t="n">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="M35" t="inlineStr">
         <is>
@@ -7076,7 +7076,7 @@
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O35" t="inlineStr">
@@ -7111,22 +7111,22 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>acowboy7</t>
+          <t>100% Amos</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>#9L0C0C82</t>
+          <t>#LYGLRCQCR</t>
         </is>
       </c>
       <c r="H36" t="n">
         <v>18</v>
       </c>
       <c r="I36" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K36" t="n">
         <v>3</v>
@@ -7176,25 +7176,25 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>100% dadeux</t>
+          <t>100% Amos</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>#PRR2RJJ9U</t>
+          <t>#LYGLRCQCR</t>
         </is>
       </c>
       <c r="H37" t="n">
         <v>18</v>
       </c>
       <c r="I37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L37" t="n">
         <v>83</v>
@@ -7241,37 +7241,37 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>100% dadeux</t>
+          <t>LittleSinn</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>#PRR2RJJ9U</t>
+          <t>#YGV99UU</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I38" t="n">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="J38" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K38" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L38" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
@@ -7306,32 +7306,32 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>stars</t>
+          <t>100% Titan</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>#JPCVU0C</t>
+          <t>#YJVLJG8U</t>
         </is>
       </c>
       <c r="H39" t="n">
         <v>18</v>
       </c>
       <c r="I39" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J39" t="n">
         <v>1</v>
       </c>
       <c r="K39" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L39" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
@@ -7371,19 +7371,19 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>stars</t>
+          <t>100% Titan</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>#JPCVU0C</t>
+          <t>#YJVLJG8U</t>
         </is>
       </c>
       <c r="H40" t="n">
         <v>18</v>
       </c>
       <c r="I40" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J40" t="n">
         <v>2</v>
@@ -7436,28 +7436,28 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Azend</t>
+          <t>acowboy7</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>#LY9GC9LJQ</t>
+          <t>#9L0C0C82</t>
         </is>
       </c>
       <c r="H41" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I41" t="n">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="J41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L41" t="n">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="M41" t="inlineStr">
         <is>
@@ -7466,7 +7466,7 @@
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O41" t="inlineStr">
@@ -7501,22 +7501,22 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>NISHANT 2.O</t>
+          <t>acowboy7</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>#9PVL282R8</t>
+          <t>#9L0C0C82</t>
         </is>
       </c>
       <c r="H42" t="n">
         <v>18</v>
       </c>
       <c r="I42" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="J42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K42" t="n">
         <v>3</v>
@@ -7566,28 +7566,28 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>NISHANT 2.O</t>
+          <t>100% dadeux</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>#9PVL282R8</t>
+          <t>#PRR2RJJ9U</t>
         </is>
       </c>
       <c r="H43" t="n">
         <v>18</v>
       </c>
       <c r="I43" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="J43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L43" t="n">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="M43" t="inlineStr">
         <is>
@@ -7631,32 +7631,32 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>100% OZI</t>
+          <t>100% dadeux</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>#9JJRCPQ08</t>
+          <t>#PRR2RJJ9U</t>
         </is>
       </c>
       <c r="H44" t="n">
         <v>18</v>
       </c>
       <c r="I44" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="J44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K44" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L44" t="n">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
@@ -7696,32 +7696,32 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>100% OZI</t>
+          <t>stars</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>#9JJRCPQ08</t>
+          <t>#JPCVU0C</t>
         </is>
       </c>
       <c r="H45" t="n">
         <v>18</v>
       </c>
       <c r="I45" t="n">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="J45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L45" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
@@ -7761,37 +7761,37 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>100% abo3bdo3mk</t>
+          <t>stars</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>#G0CCYPGCQ</t>
+          <t>#JPCVU0C</t>
         </is>
       </c>
       <c r="H46" t="n">
         <v>18</v>
       </c>
       <c r="I46" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J46" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K46" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L46" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O46" t="inlineStr">
@@ -7826,28 +7826,28 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Azend</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>#LGRPC9CYG</t>
+          <t>#LY9GC9LJQ</t>
         </is>
       </c>
       <c r="H47" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I47" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="J47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K47" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L47" t="n">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="M47" t="inlineStr">
         <is>
@@ -7856,7 +7856,7 @@
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O47" t="inlineStr">
@@ -7891,28 +7891,28 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>murph</t>
+          <t>Azend</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>#PU8L9PVJQ</t>
+          <t>#LY9GC9LJQ</t>
         </is>
       </c>
       <c r="H48" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I48" t="n">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="J48" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K48" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L48" t="n">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="M48" t="inlineStr">
         <is>
@@ -7921,7 +7921,7 @@
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O48" t="inlineStr">
@@ -7956,32 +7956,32 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>stars</t>
+          <t>NISHANT 2.O</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>#Y0UQQGYP2</t>
+          <t>#9PVL282R8</t>
         </is>
       </c>
       <c r="H49" t="n">
         <v>18</v>
       </c>
       <c r="I49" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J49" t="n">
         <v>1</v>
       </c>
       <c r="K49" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L49" t="n">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
@@ -8021,28 +8021,28 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>stars</t>
+          <t>NISHANT 2.O</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>#Y0UQQGYP2</t>
+          <t>#9PVL282R8</t>
         </is>
       </c>
       <c r="H50" t="n">
         <v>18</v>
       </c>
       <c r="I50" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J50" t="n">
         <v>2</v>
       </c>
       <c r="K50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L50" t="n">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="M50" t="inlineStr">
         <is>
@@ -8086,28 +8086,28 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>BlueberryPie</t>
+          <t>100% OZI</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>#QQGY0JYGR</t>
+          <t>#9JJRCPQ08</t>
         </is>
       </c>
       <c r="H51" t="n">
+        <v>18</v>
+      </c>
+      <c r="I51" t="n">
         <v>14</v>
-      </c>
-      <c r="I51" t="n">
-        <v>34</v>
       </c>
       <c r="J51" t="n">
         <v>1</v>
       </c>
       <c r="K51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L51" t="n">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="M51" t="inlineStr">
         <is>
@@ -8151,40 +8151,560 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
+          <t>100% OZI</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>#9JJRCPQ08</t>
+        </is>
+      </c>
+      <c r="H52" t="n">
+        <v>18</v>
+      </c>
+      <c r="I52" t="n">
+        <v>14</v>
+      </c>
+      <c r="J52" t="n">
+        <v>2</v>
+      </c>
+      <c r="K52" t="n">
+        <v>3</v>
+      </c>
+      <c r="L52" t="n">
+        <v>100</v>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>20260119T102025-000Z</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>20260121T092025.000Z</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>35</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>100% abo3bdo3mk</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>#G0CCYPGCQ</t>
+        </is>
+      </c>
+      <c r="H53" t="n">
+        <v>18</v>
+      </c>
+      <c r="I53" t="n">
+        <v>23</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0</v>
+      </c>
+      <c r="L53" t="n">
+        <v>0</v>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>20260119T102025-000Z</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>20260121T092025.000Z</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>35</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>#LGRPC9CYG</t>
+        </is>
+      </c>
+      <c r="H54" t="n">
+        <v>18</v>
+      </c>
+      <c r="I54" t="n">
+        <v>28</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0</v>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>20260119T102025-000Z</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>20260121T092025.000Z</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>35</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>murph</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>#PU8L9PVJQ</t>
+        </is>
+      </c>
+      <c r="H55" t="n">
+        <v>18</v>
+      </c>
+      <c r="I55" t="n">
+        <v>25</v>
+      </c>
+      <c r="J55" t="n">
+        <v>1</v>
+      </c>
+      <c r="K55" t="n">
+        <v>2</v>
+      </c>
+      <c r="L55" t="n">
+        <v>82</v>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>20260119T102025-000Z</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>20260121T092025.000Z</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>35</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>murph</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>#PU8L9PVJQ</t>
+        </is>
+      </c>
+      <c r="H56" t="n">
+        <v>18</v>
+      </c>
+      <c r="I56" t="n">
+        <v>25</v>
+      </c>
+      <c r="J56" t="n">
+        <v>2</v>
+      </c>
+      <c r="K56" t="n">
+        <v>2</v>
+      </c>
+      <c r="L56" t="n">
+        <v>62</v>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>20260119T102025-000Z</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>20260121T092025.000Z</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>35</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>stars</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>#Y0UQQGYP2</t>
+        </is>
+      </c>
+      <c r="H57" t="n">
+        <v>18</v>
+      </c>
+      <c r="I57" t="n">
+        <v>22</v>
+      </c>
+      <c r="J57" t="n">
+        <v>1</v>
+      </c>
+      <c r="K57" t="n">
+        <v>1</v>
+      </c>
+      <c r="L57" t="n">
+        <v>2</v>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>20260119T102025-000Z</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>20260121T092025.000Z</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>35</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>stars</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>#Y0UQQGYP2</t>
+        </is>
+      </c>
+      <c r="H58" t="n">
+        <v>18</v>
+      </c>
+      <c r="I58" t="n">
+        <v>22</v>
+      </c>
+      <c r="J58" t="n">
+        <v>2</v>
+      </c>
+      <c r="K58" t="n">
+        <v>1</v>
+      </c>
+      <c r="L58" t="n">
+        <v>47</v>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>20260119T102025-000Z</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>20260121T092025.000Z</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>35</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
           <t>BlueberryPie</t>
         </is>
       </c>
-      <c r="G52" t="inlineStr">
+      <c r="G59" t="inlineStr">
         <is>
           <t>#QQGY0JYGR</t>
         </is>
       </c>
-      <c r="H52" t="n">
+      <c r="H59" t="n">
         <v>14</v>
       </c>
-      <c r="I52" t="n">
+      <c r="I59" t="n">
         <v>34</v>
       </c>
-      <c r="J52" t="n">
-        <v>2</v>
-      </c>
-      <c r="K52" t="n">
-        <v>2</v>
-      </c>
-      <c r="L52" t="n">
+      <c r="J59" t="n">
+        <v>1</v>
+      </c>
+      <c r="K59" t="n">
+        <v>2</v>
+      </c>
+      <c r="L59" t="n">
+        <v>61</v>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>20260119T102025-000Z</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>20260121T092025.000Z</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>35</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>BlueberryPie</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>#QQGY0JYGR</t>
+        </is>
+      </c>
+      <c r="H60" t="n">
+        <v>14</v>
+      </c>
+      <c r="I60" t="n">
+        <v>34</v>
+      </c>
+      <c r="J60" t="n">
+        <v>2</v>
+      </c>
+      <c r="K60" t="n">
+        <v>2</v>
+      </c>
+      <c r="L60" t="n">
         <v>50</v>
       </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="N52" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="O52" t="inlineStr">
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr">
         <is>
           <t>No</t>
         </is>

</xml_diff>

<commit_message>
Fix avg stars display, add missed hits back, improve spacing
</commit_message>
<xml_diff>
--- a/clash_wars.xlsx
+++ b/clash_wars.xlsx
@@ -959,7 +959,7 @@
         <v>2</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
@@ -4773,7 +4773,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O60"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7061,22 +7061,22 @@
         <v>31</v>
       </c>
       <c r="J35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L35" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O35" t="inlineStr">
@@ -7111,22 +7111,22 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>100% Amos</t>
+          <t>Mr Owl</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>#LYGLRCQCR</t>
+          <t>#LQ8CU8GPU</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I36" t="n">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="J36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K36" t="n">
         <v>3</v>
@@ -7191,17 +7191,17 @@
         <v>7</v>
       </c>
       <c r="J37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K37" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L37" t="n">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
@@ -7241,28 +7241,28 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>LittleSinn</t>
+          <t>100% Amos</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>#YGV99UU</t>
+          <t>#LYGLRCQCR</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I38" t="n">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="J38" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K38" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L38" t="n">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="M38" t="inlineStr">
         <is>
@@ -7271,7 +7271,7 @@
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
@@ -7306,37 +7306,37 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>100% Titan</t>
+          <t>LittleSinn</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>#YJVLJG8U</t>
+          <t>#YGV99UU</t>
         </is>
       </c>
       <c r="H39" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I39" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K39" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L39" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O39" t="inlineStr">
@@ -7386,7 +7386,7 @@
         <v>26</v>
       </c>
       <c r="J40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K40" t="n">
         <v>3</v>
@@ -7436,32 +7436,32 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>acowboy7</t>
+          <t>100% Titan</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>#9L0C0C82</t>
+          <t>#YJVLJG8U</t>
         </is>
       </c>
       <c r="H41" t="n">
         <v>18</v>
       </c>
       <c r="I41" t="n">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="J41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K41" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L41" t="n">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
@@ -7516,17 +7516,17 @@
         <v>6</v>
       </c>
       <c r="J42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K42" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L42" t="n">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
@@ -7566,32 +7566,32 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>100% dadeux</t>
+          <t>acowboy7</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>#PRR2RJJ9U</t>
+          <t>#9L0C0C82</t>
         </is>
       </c>
       <c r="H43" t="n">
         <v>18</v>
       </c>
       <c r="I43" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K43" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L43" t="n">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
@@ -7646,17 +7646,17 @@
         <v>8</v>
       </c>
       <c r="J44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K44" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L44" t="n">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
@@ -7696,32 +7696,32 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>stars</t>
+          <t>100% dadeux</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>#JPCVU0C</t>
+          <t>#PRR2RJJ9U</t>
         </is>
       </c>
       <c r="H45" t="n">
         <v>18</v>
       </c>
       <c r="I45" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="J45" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K45" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L45" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
@@ -7776,17 +7776,17 @@
         <v>24</v>
       </c>
       <c r="J46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L46" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
@@ -7826,32 +7826,32 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Azend</t>
+          <t>stars</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>#LY9GC9LJQ</t>
+          <t>#JPCVU0C</t>
         </is>
       </c>
       <c r="H47" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I47" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="J47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K47" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L47" t="n">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
@@ -7906,13 +7906,13 @@
         <v>32</v>
       </c>
       <c r="J48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K48" t="n">
         <v>2</v>
       </c>
       <c r="L48" t="n">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="M48" t="inlineStr">
         <is>
@@ -7956,32 +7956,32 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>NISHANT 2.O</t>
+          <t>Azend</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>#9PVL282R8</t>
+          <t>#LY9GC9LJQ</t>
         </is>
       </c>
       <c r="H49" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I49" t="n">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="J49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L49" t="n">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
@@ -8036,17 +8036,17 @@
         <v>15</v>
       </c>
       <c r="J50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K50" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L50" t="n">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
@@ -8086,28 +8086,28 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>100% OZI</t>
+          <t>NISHANT 2.O</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>#9JJRCPQ08</t>
+          <t>#9PVL282R8</t>
         </is>
       </c>
       <c r="H51" t="n">
         <v>18</v>
       </c>
       <c r="I51" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L51" t="n">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="M51" t="inlineStr">
         <is>
@@ -8166,17 +8166,17 @@
         <v>14</v>
       </c>
       <c r="J52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K52" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L52" t="n">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
@@ -8216,37 +8216,37 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>100% abo3bdo3mk</t>
+          <t>100% OZI</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>#G0CCYPGCQ</t>
+          <t>#9JJRCPQ08</t>
         </is>
       </c>
       <c r="H53" t="n">
         <v>18</v>
       </c>
       <c r="I53" t="n">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="J53" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K53" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L53" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O53" t="inlineStr">
@@ -8281,19 +8281,19 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>100% abo3bdo3mk</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>#LGRPC9CYG</t>
+          <t>#G0CCYPGCQ</t>
         </is>
       </c>
       <c r="H54" t="n">
         <v>18</v>
       </c>
       <c r="I54" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="J54" t="n">
         <v>0</v>
@@ -8346,28 +8346,28 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>murph</t>
+          <t>John</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>#PU8L9PVJQ</t>
+          <t>#LGRPC9CYG</t>
         </is>
       </c>
       <c r="H55" t="n">
         <v>18</v>
       </c>
       <c r="I55" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K55" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L55" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="M55" t="inlineStr">
         <is>
@@ -8376,7 +8376,7 @@
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O55" t="inlineStr">
@@ -8426,13 +8426,13 @@
         <v>25</v>
       </c>
       <c r="J56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K56" t="n">
         <v>2</v>
       </c>
       <c r="L56" t="n">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="M56" t="inlineStr">
         <is>
@@ -8476,28 +8476,28 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>stars</t>
+          <t>murph</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>#Y0UQQGYP2</t>
+          <t>#PU8L9PVJQ</t>
         </is>
       </c>
       <c r="H57" t="n">
         <v>18</v>
       </c>
       <c r="I57" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J57" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K57" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L57" t="n">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="M57" t="inlineStr">
         <is>
@@ -8556,13 +8556,13 @@
         <v>22</v>
       </c>
       <c r="J58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K58" t="n">
         <v>1</v>
       </c>
       <c r="L58" t="n">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="M58" t="inlineStr">
         <is>
@@ -8606,28 +8606,28 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>BlueberryPie</t>
+          <t>stars</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>#QQGY0JYGR</t>
+          <t>#Y0UQQGYP2</t>
         </is>
       </c>
       <c r="H59" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I59" t="n">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="J59" t="n">
+        <v>2</v>
+      </c>
+      <c r="K59" t="n">
         <v>1</v>
       </c>
-      <c r="K59" t="n">
-        <v>2</v>
-      </c>
       <c r="L59" t="n">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="M59" t="inlineStr">
         <is>
@@ -8686,25 +8686,90 @@
         <v>34</v>
       </c>
       <c r="J60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K60" t="n">
         <v>2</v>
       </c>
       <c r="L60" t="n">
+        <v>61</v>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>20260119T102025-000Z</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>20260121T092025.000Z</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>35</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>BlueberryPie</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>#QQGY0JYGR</t>
+        </is>
+      </c>
+      <c r="H61" t="n">
+        <v>14</v>
+      </c>
+      <c r="I61" t="n">
+        <v>34</v>
+      </c>
+      <c r="J61" t="n">
+        <v>2</v>
+      </c>
+      <c r="K61" t="n">
+        <v>2</v>
+      </c>
+      <c r="L61" t="n">
         <v>50</v>
       </c>
-      <c r="M60" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="N60" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="O60" t="inlineStr">
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O61" t="inlineStr">
         <is>
           <t>No</t>
         </is>

</xml_diff>

<commit_message>
Sort by 3-star rate, show avg stars instead of total
</commit_message>
<xml_diff>
--- a/clash_wars.xlsx
+++ b/clash_wars.xlsx
@@ -938,7 +938,7 @@
         <v>2</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
@@ -7321,22 +7321,22 @@
         <v>30</v>
       </c>
       <c r="J39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K39" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L39" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O39" t="inlineStr">

</xml_diff>

<commit_message>
Fix average stars calculation - now per attack not per war
</commit_message>
<xml_diff>
--- a/clash_wars.xlsx
+++ b/clash_wars.xlsx
@@ -917,7 +917,7 @@
         <v>2</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -938,7 +938,7 @@
         <v>2</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
@@ -4773,7 +4773,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6801,22 +6801,22 @@
         <v>18</v>
       </c>
       <c r="J31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L31" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
@@ -7371,32 +7371,32 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>100% Titan</t>
+          <t>LittleSinn</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>#YJVLJG8U</t>
+          <t>#YGV99UU</t>
         </is>
       </c>
       <c r="H40" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I40" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L40" t="n">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
@@ -7451,7 +7451,7 @@
         <v>26</v>
       </c>
       <c r="J41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K41" t="n">
         <v>3</v>
@@ -7501,32 +7501,32 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>acowboy7</t>
+          <t>100% Titan</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>#9L0C0C82</t>
+          <t>#YJVLJG8U</t>
         </is>
       </c>
       <c r="H42" t="n">
         <v>18</v>
       </c>
       <c r="I42" t="n">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="J42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K42" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L42" t="n">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
@@ -7581,17 +7581,17 @@
         <v>6</v>
       </c>
       <c r="J43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K43" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L43" t="n">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
@@ -7631,32 +7631,32 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>100% dadeux</t>
+          <t>acowboy7</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>#PRR2RJJ9U</t>
+          <t>#9L0C0C82</t>
         </is>
       </c>
       <c r="H44" t="n">
         <v>18</v>
       </c>
       <c r="I44" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K44" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L44" t="n">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
@@ -7711,17 +7711,17 @@
         <v>8</v>
       </c>
       <c r="J45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K45" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L45" t="n">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
@@ -7761,32 +7761,32 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>stars</t>
+          <t>100% dadeux</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>#JPCVU0C</t>
+          <t>#PRR2RJJ9U</t>
         </is>
       </c>
       <c r="H46" t="n">
         <v>18</v>
       </c>
       <c r="I46" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="J46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K46" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L46" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
@@ -7841,17 +7841,17 @@
         <v>24</v>
       </c>
       <c r="J47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L47" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
@@ -7891,32 +7891,32 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Azend</t>
+          <t>stars</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>#LY9GC9LJQ</t>
+          <t>#JPCVU0C</t>
         </is>
       </c>
       <c r="H48" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I48" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="J48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K48" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L48" t="n">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
@@ -7971,13 +7971,13 @@
         <v>32</v>
       </c>
       <c r="J49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K49" t="n">
         <v>2</v>
       </c>
       <c r="L49" t="n">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="M49" t="inlineStr">
         <is>
@@ -8021,32 +8021,32 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>NISHANT 2.O</t>
+          <t>Azend</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>#9PVL282R8</t>
+          <t>#LY9GC9LJQ</t>
         </is>
       </c>
       <c r="H50" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I50" t="n">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="J50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L50" t="n">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
@@ -8101,17 +8101,17 @@
         <v>15</v>
       </c>
       <c r="J51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L51" t="n">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
@@ -8151,28 +8151,28 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>100% OZI</t>
+          <t>NISHANT 2.O</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>#9JJRCPQ08</t>
+          <t>#9PVL282R8</t>
         </is>
       </c>
       <c r="H52" t="n">
         <v>18</v>
       </c>
       <c r="I52" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J52" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K52" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L52" t="n">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="M52" t="inlineStr">
         <is>
@@ -8231,17 +8231,17 @@
         <v>14</v>
       </c>
       <c r="J53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K53" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L53" t="n">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
@@ -8281,37 +8281,37 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>100% abo3bdo3mk</t>
+          <t>100% OZI</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>#G0CCYPGCQ</t>
+          <t>#9JJRCPQ08</t>
         </is>
       </c>
       <c r="H54" t="n">
         <v>18</v>
       </c>
       <c r="I54" t="n">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="J54" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K54" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L54" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O54" t="inlineStr">
@@ -8346,19 +8346,19 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>100% abo3bdo3mk</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>#LGRPC9CYG</t>
+          <t>#G0CCYPGCQ</t>
         </is>
       </c>
       <c r="H55" t="n">
         <v>18</v>
       </c>
       <c r="I55" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="J55" t="n">
         <v>0</v>
@@ -8411,28 +8411,28 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>murph</t>
+          <t>John</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>#PU8L9PVJQ</t>
+          <t>#LGRPC9CYG</t>
         </is>
       </c>
       <c r="H56" t="n">
         <v>18</v>
       </c>
       <c r="I56" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K56" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L56" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="M56" t="inlineStr">
         <is>
@@ -8441,7 +8441,7 @@
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O56" t="inlineStr">
@@ -8491,13 +8491,13 @@
         <v>25</v>
       </c>
       <c r="J57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K57" t="n">
         <v>2</v>
       </c>
       <c r="L57" t="n">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="M57" t="inlineStr">
         <is>
@@ -8541,28 +8541,28 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>stars</t>
+          <t>murph</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>#Y0UQQGYP2</t>
+          <t>#PU8L9PVJQ</t>
         </is>
       </c>
       <c r="H58" t="n">
         <v>18</v>
       </c>
       <c r="I58" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L58" t="n">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="M58" t="inlineStr">
         <is>
@@ -8621,13 +8621,13 @@
         <v>22</v>
       </c>
       <c r="J59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K59" t="n">
         <v>1</v>
       </c>
       <c r="L59" t="n">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="M59" t="inlineStr">
         <is>
@@ -8671,28 +8671,28 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>BlueberryPie</t>
+          <t>stars</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>#QQGY0JYGR</t>
+          <t>#Y0UQQGYP2</t>
         </is>
       </c>
       <c r="H60" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I60" t="n">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="J60" t="n">
+        <v>2</v>
+      </c>
+      <c r="K60" t="n">
         <v>1</v>
       </c>
-      <c r="K60" t="n">
-        <v>2</v>
-      </c>
       <c r="L60" t="n">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="M60" t="inlineStr">
         <is>
@@ -8751,25 +8751,90 @@
         <v>34</v>
       </c>
       <c r="J61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K61" t="n">
         <v>2</v>
       </c>
       <c r="L61" t="n">
+        <v>61</v>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>20260119T102025-000Z</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>20260121T092025.000Z</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>35</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>BlueberryPie</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>#QQGY0JYGR</t>
+        </is>
+      </c>
+      <c r="H62" t="n">
+        <v>14</v>
+      </c>
+      <c r="I62" t="n">
+        <v>34</v>
+      </c>
+      <c r="J62" t="n">
+        <v>2</v>
+      </c>
+      <c r="K62" t="n">
+        <v>2</v>
+      </c>
+      <c r="L62" t="n">
         <v>50</v>
       </c>
-      <c r="M61" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="N61" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="O61" t="inlineStr">
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr">
         <is>
           <t>No</t>
         </is>

</xml_diff>

<commit_message>
Fix war participation for players with missed hits, add total stars
</commit_message>
<xml_diff>
--- a/clash_wars.xlsx
+++ b/clash_wars.xlsx
@@ -573,7 +573,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -594,7 +594,7 @@
         <v>3</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -678,7 +678,7 @@
         <v>3</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
@@ -699,7 +699,7 @@
         <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
@@ -720,7 +720,7 @@
         <v>3</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12">
@@ -783,7 +783,7 @@
         <v>3</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
@@ -825,7 +825,7 @@
         <v>3</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
@@ -846,7 +846,7 @@
         <v>3</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
@@ -867,7 +867,7 @@
         <v>3</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -909,7 +909,7 @@
         <v>3</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21">
@@ -1014,7 +1014,7 @@
         <v>3</v>
       </c>
       <c r="E25" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26">
@@ -1161,7 +1161,7 @@
         <v>3</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33">
@@ -1266,7 +1266,7 @@
         <v>3</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
@@ -1287,7 +1287,7 @@
         <v>3</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -9344,7 +9344,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9487,22 +9487,22 @@
         <v>13</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -9537,37 +9537,37 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>100% Meli</t>
+          <t>EvlGniz</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>#99QUJCCYJ</t>
+          <t>#8G8VV89JJ</t>
         </is>
       </c>
       <c r="H3" t="n">
         <v>18</v>
       </c>
       <c r="I3" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -9602,19 +9602,19 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>100% Rogers</t>
+          <t>100% Meli</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>#Q9UPUUGRL</t>
+          <t>#99QUJCCYJ</t>
         </is>
       </c>
       <c r="H4" t="n">
         <v>18</v>
       </c>
       <c r="I4" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
@@ -9667,28 +9667,28 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Downsy m8</t>
+          <t>100% Rogers</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>#PYR0JQC</t>
+          <t>#Q9UPUUGRL</t>
         </is>
       </c>
       <c r="H5" t="n">
         <v>18</v>
       </c>
       <c r="I5" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
@@ -9697,7 +9697,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -9732,37 +9732,37 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Anon</t>
+          <t>100% Rogers</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>#2VRP9CJY</t>
+          <t>#Q9UPUUGRL</t>
         </is>
       </c>
       <c r="H6" t="n">
         <v>18</v>
       </c>
       <c r="I6" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -9797,37 +9797,37 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>«#PATRICK#»</t>
+          <t>Downsy m8</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>#8R8R0GL9</t>
+          <t>#PYR0JQC</t>
         </is>
       </c>
       <c r="H7" t="n">
         <v>18</v>
       </c>
       <c r="I7" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
@@ -9862,37 +9862,37 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Frodo</t>
+          <t>Downsy m8</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>#282Q98Y9J</t>
+          <t>#PYR0JQC</t>
         </is>
       </c>
       <c r="H8" t="n">
         <v>18</v>
       </c>
       <c r="I8" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
@@ -9927,37 +9927,37 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>stars2</t>
+          <t>Anon</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>#YJC80V2QC</t>
+          <t>#2VRP9CJY</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I9" t="n">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
@@ -9992,37 +9992,37 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Innersinn</t>
+          <t>Anon</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>#9UUG9GPC</t>
+          <t>#2VRP9CJY</t>
         </is>
       </c>
       <c r="H10" t="n">
         <v>18</v>
       </c>
       <c r="I10" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -10057,37 +10057,37 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>zZz • Iztelikk</t>
+          <t>«#PATRICK#»</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>#8PUV2Q0C0</t>
+          <t>#8R8R0GL9</t>
         </is>
       </c>
       <c r="H11" t="n">
         <v>18</v>
       </c>
       <c r="I11" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
@@ -10122,22 +10122,22 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>platypus</t>
+          <t>«#PATRICK#»</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>#VQUQ8992</t>
+          <t>#8R8R0GL9</t>
         </is>
       </c>
       <c r="H12" t="n">
         <v>18</v>
       </c>
       <c r="I12" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12" t="n">
         <v>3</v>
@@ -10187,37 +10187,37 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>BlueberyPancake</t>
+          <t>Frodo</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>#G2PQRR0QV</t>
+          <t>#282Q98Y9J</t>
         </is>
       </c>
       <c r="H13" t="n">
         <v>18</v>
       </c>
       <c r="I13" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
@@ -10252,19 +10252,19 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>100% dado</t>
+          <t>stars2</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>#8G89CPJVU</t>
+          <t>#YJC80V2QC</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
@@ -10317,37 +10317,37 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>savage slayer</t>
+          <t>Innersinn</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>#YGY8R0YV8</t>
+          <t>#9UUG9GPC</t>
         </is>
       </c>
       <c r="H15" t="n">
         <v>18</v>
       </c>
       <c r="I15" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -10382,28 +10382,28 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>abhi</t>
+          <t>Innersinn</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>#P8Y9JR8CP</t>
+          <t>#9UUG9GPC</t>
         </is>
       </c>
       <c r="H16" t="n">
         <v>18</v>
       </c>
       <c r="I16" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="M16" t="inlineStr">
         <is>
@@ -10412,7 +10412,7 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -10447,28 +10447,28 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Krunal</t>
+          <t>zZz • Iztelikk</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>#8VC29JPJP</t>
+          <t>#8PUV2Q0C0</t>
         </is>
       </c>
       <c r="H17" t="n">
         <v>18</v>
       </c>
       <c r="I17" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" t="n">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="M17" t="inlineStr">
         <is>
@@ -10477,7 +10477,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -10512,28 +10512,28 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>TN • Raiden</t>
+          <t>zZz • Iztelikk</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>#GV90C0LU</t>
+          <t>#8PUV2Q0C0</t>
         </is>
       </c>
       <c r="H18" t="n">
         <v>18</v>
       </c>
       <c r="I18" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="J18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L18" t="n">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="M18" t="inlineStr">
         <is>
@@ -10542,7 +10542,7 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
@@ -10577,37 +10577,37 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Mr Owl</t>
+          <t>platypus</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>#LQ8CU8GPU</t>
+          <t>#VQUQ8992</t>
         </is>
       </c>
       <c r="H19" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I19" t="n">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L19" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
@@ -10642,28 +10642,28 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>100% Amos</t>
+          <t>BlueberyPancake</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>#LYGLRCQCR</t>
+          <t>#G2PQRR0QV</t>
         </is>
       </c>
       <c r="H20" t="n">
         <v>18</v>
       </c>
       <c r="I20" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L20" t="n">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="M20" t="inlineStr">
         <is>
@@ -10672,7 +10672,7 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
@@ -10707,37 +10707,37 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>LittleSinn</t>
+          <t>BlueberyPancake</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>#YGV99UU</t>
+          <t>#G2PQRR0QV</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I21" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L21" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
@@ -10772,19 +10772,19 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>100% Titan</t>
+          <t>100% dado</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>#YJVLJG8U</t>
+          <t>#8G89CPJVU</t>
         </is>
       </c>
       <c r="H22" t="n">
         <v>18</v>
       </c>
       <c r="I22" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="J22" t="n">
         <v>1</v>
@@ -10837,19 +10837,19 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>100% Titan</t>
+          <t>100% dado</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>#YJVLJG8U</t>
+          <t>#8G89CPJVU</t>
         </is>
       </c>
       <c r="H23" t="n">
         <v>18</v>
       </c>
       <c r="I23" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="J23" t="n">
         <v>2</v>
@@ -10902,19 +10902,19 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>acowboy7</t>
+          <t>savage slayer</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>#9L0C0C82</t>
+          <t>#YGY8R0YV8</t>
         </is>
       </c>
       <c r="H24" t="n">
         <v>18</v>
       </c>
       <c r="I24" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="J24" t="n">
         <v>0</v>
@@ -10967,19 +10967,19 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>100% dadeux</t>
+          <t>abhi</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>#PRR2RJJ9U</t>
+          <t>#P8Y9JR8CP</t>
         </is>
       </c>
       <c r="H25" t="n">
         <v>18</v>
       </c>
       <c r="I25" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="J25" t="n">
         <v>0</v>
@@ -11032,37 +11032,37 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>stars</t>
+          <t>Krunal</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>#JPCVU0C</t>
+          <t>#8VC29JPJP</t>
         </is>
       </c>
       <c r="H26" t="n">
         <v>18</v>
       </c>
       <c r="I26" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L26" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
@@ -11097,37 +11097,37 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>stars</t>
+          <t>TN • Raiden</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>#JPCVU0C</t>
+          <t>#GV90C0LU</t>
         </is>
       </c>
       <c r="H27" t="n">
         <v>18</v>
       </c>
       <c r="I27" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J27" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L27" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
@@ -11162,37 +11162,37 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Azend</t>
+          <t>Mr Owl</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>#LY9GC9LJQ</t>
+          <t>#LQ8CU8GPU</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I28" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L28" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
@@ -11227,28 +11227,28 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Azend</t>
+          <t>100% Amos</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>#LY9GC9LJQ</t>
+          <t>#LYGLRCQCR</t>
         </is>
       </c>
       <c r="H29" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I29" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="J29" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K29" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L29" t="n">
-        <v>93</v>
+        <v>0</v>
       </c>
       <c r="M29" t="inlineStr">
         <is>
@@ -11257,7 +11257,7 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
@@ -11292,19 +11292,19 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>NISHANT 2.O</t>
+          <t>LittleSinn</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>#9PVL282R8</t>
+          <t>#YGV99UU</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I30" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="J30" t="n">
         <v>0</v>
@@ -11357,37 +11357,37 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>polomanino</t>
+          <t>100% Titan</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>#GCLRRVYP</t>
+          <t>#YJVLJG8U</t>
         </is>
       </c>
       <c r="H31" t="n">
         <v>18</v>
       </c>
       <c r="I31" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="J31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L31" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
@@ -11422,37 +11422,37 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>100% OZI</t>
+          <t>100% Titan</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>#9JJRCPQ08</t>
+          <t>#YJVLJG8U</t>
         </is>
       </c>
       <c r="H32" t="n">
         <v>18</v>
       </c>
       <c r="I32" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="J32" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K32" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L32" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O32" t="inlineStr">
@@ -11487,19 +11487,19 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>acowboy7</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>#LGRPC9CYG</t>
+          <t>#9L0C0C82</t>
         </is>
       </c>
       <c r="H33" t="n">
         <v>18</v>
       </c>
       <c r="I33" t="n">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="J33" t="n">
         <v>0</v>
@@ -11552,28 +11552,28 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>murph</t>
+          <t>100% dadeux</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>#PU8L9PVJQ</t>
+          <t>#PRR2RJJ9U</t>
         </is>
       </c>
       <c r="H34" t="n">
         <v>18</v>
       </c>
       <c r="I34" t="n">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="J34" t="n">
         <v>1</v>
       </c>
       <c r="K34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L34" t="n">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="M34" t="inlineStr">
         <is>
@@ -11617,40 +11617,885 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
+          <t>100% dadeux</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>#PRR2RJJ9U</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>18</v>
+      </c>
+      <c r="I35" t="n">
+        <v>5</v>
+      </c>
+      <c r="J35" t="n">
+        <v>2</v>
+      </c>
+      <c r="K35" t="n">
+        <v>2</v>
+      </c>
+      <c r="L35" t="n">
+        <v>81</v>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>20260121T092201-000Z</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>20260123T082201.000Z</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>30</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>stars</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>#JPCVU0C</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>18</v>
+      </c>
+      <c r="I36" t="n">
+        <v>22</v>
+      </c>
+      <c r="J36" t="n">
+        <v>1</v>
+      </c>
+      <c r="K36" t="n">
+        <v>3</v>
+      </c>
+      <c r="L36" t="n">
+        <v>100</v>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>20260121T092201-000Z</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>20260123T082201.000Z</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>30</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>stars</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>#JPCVU0C</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>18</v>
+      </c>
+      <c r="I37" t="n">
+        <v>22</v>
+      </c>
+      <c r="J37" t="n">
+        <v>2</v>
+      </c>
+      <c r="K37" t="n">
+        <v>3</v>
+      </c>
+      <c r="L37" t="n">
+        <v>100</v>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>20260121T092201-000Z</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>20260123T082201.000Z</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>30</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Azend</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>#LY9GC9LJQ</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>15</v>
+      </c>
+      <c r="I38" t="n">
+        <v>30</v>
+      </c>
+      <c r="J38" t="n">
+        <v>1</v>
+      </c>
+      <c r="K38" t="n">
+        <v>3</v>
+      </c>
+      <c r="L38" t="n">
+        <v>100</v>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>20260121T092201-000Z</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>20260123T082201.000Z</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>30</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Azend</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>#LY9GC9LJQ</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>15</v>
+      </c>
+      <c r="I39" t="n">
+        <v>30</v>
+      </c>
+      <c r="J39" t="n">
+        <v>2</v>
+      </c>
+      <c r="K39" t="n">
+        <v>2</v>
+      </c>
+      <c r="L39" t="n">
+        <v>93</v>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>20260121T092201-000Z</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>20260123T082201.000Z</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>30</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>NISHANT 2.O</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>#9PVL282R8</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>18</v>
+      </c>
+      <c r="I40" t="n">
+        <v>14</v>
+      </c>
+      <c r="J40" t="n">
+        <v>1</v>
+      </c>
+      <c r="K40" t="n">
+        <v>3</v>
+      </c>
+      <c r="L40" t="n">
+        <v>100</v>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>20260121T092201-000Z</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>20260123T082201.000Z</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>30</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>NISHANT 2.O</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>#9PVL282R8</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>18</v>
+      </c>
+      <c r="I41" t="n">
+        <v>14</v>
+      </c>
+      <c r="J41" t="n">
+        <v>2</v>
+      </c>
+      <c r="K41" t="n">
+        <v>3</v>
+      </c>
+      <c r="L41" t="n">
+        <v>100</v>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>20260121T092201-000Z</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>20260123T082201.000Z</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>30</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>polomanino</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>#GCLRRVYP</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
+        <v>18</v>
+      </c>
+      <c r="I42" t="n">
+        <v>18</v>
+      </c>
+      <c r="J42" t="n">
+        <v>1</v>
+      </c>
+      <c r="K42" t="n">
+        <v>3</v>
+      </c>
+      <c r="L42" t="n">
+        <v>100</v>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>20260121T092201-000Z</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>20260123T082201.000Z</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>30</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>polomanino</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>#GCLRRVYP</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
+        <v>18</v>
+      </c>
+      <c r="I43" t="n">
+        <v>18</v>
+      </c>
+      <c r="J43" t="n">
+        <v>2</v>
+      </c>
+      <c r="K43" t="n">
+        <v>2</v>
+      </c>
+      <c r="L43" t="n">
+        <v>93</v>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>20260121T092201-000Z</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>20260123T082201.000Z</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>30</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>100% OZI</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>#9JJRCPQ08</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>18</v>
+      </c>
+      <c r="I44" t="n">
+        <v>12</v>
+      </c>
+      <c r="J44" t="n">
+        <v>1</v>
+      </c>
+      <c r="K44" t="n">
+        <v>3</v>
+      </c>
+      <c r="L44" t="n">
+        <v>100</v>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>20260121T092201-000Z</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>20260123T082201.000Z</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>30</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>100% OZI</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>#9JJRCPQ08</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>18</v>
+      </c>
+      <c r="I45" t="n">
+        <v>12</v>
+      </c>
+      <c r="J45" t="n">
+        <v>2</v>
+      </c>
+      <c r="K45" t="n">
+        <v>3</v>
+      </c>
+      <c r="L45" t="n">
+        <v>100</v>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>20260121T092201-000Z</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>20260123T082201.000Z</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>30</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>#LGRPC9CYG</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>18</v>
+      </c>
+      <c r="I46" t="n">
+        <v>26</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>20260121T092201-000Z</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>20260123T082201.000Z</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>30</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
           <t>murph</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr">
+      <c r="G47" t="inlineStr">
         <is>
           <t>#PU8L9PVJQ</t>
         </is>
       </c>
-      <c r="H35" t="n">
-        <v>18</v>
-      </c>
-      <c r="I35" t="n">
+      <c r="H47" t="n">
+        <v>18</v>
+      </c>
+      <c r="I47" t="n">
         <v>23</v>
       </c>
-      <c r="J35" t="n">
-        <v>2</v>
-      </c>
-      <c r="K35" t="n">
-        <v>2</v>
-      </c>
-      <c r="L35" t="n">
+      <c r="J47" t="n">
+        <v>1</v>
+      </c>
+      <c r="K47" t="n">
+        <v>2</v>
+      </c>
+      <c r="L47" t="n">
+        <v>91</v>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>20260121T092201-000Z</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>inWar</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>20260123T082201.000Z</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>30</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>murph</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>#PU8L9PVJQ</t>
+        </is>
+      </c>
+      <c r="H48" t="n">
+        <v>18</v>
+      </c>
+      <c r="I48" t="n">
+        <v>23</v>
+      </c>
+      <c r="J48" t="n">
+        <v>2</v>
+      </c>
+      <c r="K48" t="n">
+        <v>2</v>
+      </c>
+      <c r="L48" t="n">
         <v>92</v>
       </c>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="N35" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="O35" t="inlineStr">
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
         <is>
           <t>No</t>
         </is>

</xml_diff>